<commit_message>
verify if system can take float inputs
</commit_message>
<xml_diff>
--- a/upload_files/RTM_config.xlsx
+++ b/upload_files/RTM_config.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen.Garden\RTM\upload_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E944F32-5CDD-4072-A72D-3BBA51D6B6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Config"/>
-    <sheet r:id="rId2" sheetId="2" name="Steps"/>
+    <sheet name="Config" sheetId="1" r:id="rId1"/>
+    <sheet name="Steps" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
   <si>
     <t>Step</t>
   </si>
@@ -78,15 +84,6 @@
   </si>
   <si>
     <t>power.</t>
-  </si>
-  <si>
-    <t>Test:</t>
-  </si>
-  <si>
-    <t>SEW Highly Dynamic Test 5.1.2</t>
-  </si>
-  <si>
-    <t>70°C</t>
   </si>
   <si>
     <t>CCW</t>
@@ -113,8 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -164,35 +160,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -203,10 +204,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -244,71 +245,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -336,7 +337,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -359,11 +360,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -372,13 +373,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -388,7 +389,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -397,7 +398,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -406,7 +407,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -414,10 +415,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -482,51 +483,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="5" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="6" t="s">
+    </row>
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>800</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1">
         <v>200</v>
       </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -534,27 +587,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="4" width="12.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -573,10 +626,8 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    </row>
+    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -595,556 +646,486 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    </row>
+    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="7">
         <v>1000</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="7">
         <v>500</v>
       </c>
-      <c r="F3" s="1">
-        <v>2</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="F3" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="7">
         <v>300</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
-        <v>350</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="E4" s="7">
+        <v>350</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="7">
         <v>1000</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1">
-        <v>350</v>
-      </c>
-      <c r="F5" s="1">
-        <v>2</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="E5" s="7">
+        <v>350</v>
+      </c>
+      <c r="F5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="7">
         <v>300</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1">
-        <v>350</v>
-      </c>
-      <c r="F6" s="1">
-        <v>2</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="E6" s="7">
+        <v>350</v>
+      </c>
+      <c r="F6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="7">
         <v>1000</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="1">
-        <v>350</v>
-      </c>
-      <c r="F7" s="1">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="E7" s="7">
+        <v>350</v>
+      </c>
+      <c r="F7" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="7">
         <v>300</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1">
-        <v>350</v>
-      </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="E8" s="7">
+        <v>350</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="7">
         <v>1000</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="1">
-        <v>350</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="E9" s="7">
+        <v>350</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="7">
         <v>300</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="1">
-        <v>350</v>
-      </c>
-      <c r="F10" s="1">
-        <v>2</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="E10" s="7">
+        <v>350</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="7">
         <v>1000</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="1">
-        <v>350</v>
-      </c>
-      <c r="F11" s="1">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="E11" s="7">
+        <v>350</v>
+      </c>
+      <c r="F11" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="7">
         <v>300</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="1">
-        <v>350</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="E12" s="7">
+        <v>350</v>
+      </c>
+      <c r="F12" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="7">
         <v>800</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="7">
         <v>500</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="7">
         <v>11</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    </row>
+    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="7">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="7">
         <v>800</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="7">
         <v>11</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    </row>
+    <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="7">
         <v>1000</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="1">
+        <v>21</v>
+      </c>
+      <c r="E15" s="7">
         <v>500</v>
       </c>
-      <c r="F15" s="1">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="F15" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="7">
         <v>300</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E16" s="1">
-        <v>350</v>
-      </c>
-      <c r="F16" s="1">
-        <v>2</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+        <v>21</v>
+      </c>
+      <c r="E16" s="7">
+        <v>350</v>
+      </c>
+      <c r="F16" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="7">
         <v>1000</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="1">
-        <v>350</v>
-      </c>
-      <c r="F17" s="1">
-        <v>2</v>
-      </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+        <v>21</v>
+      </c>
+      <c r="E17" s="7">
+        <v>350</v>
+      </c>
+      <c r="F17" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="7">
         <v>300</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="1">
-        <v>350</v>
-      </c>
-      <c r="F18" s="1">
-        <v>2</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+        <v>21</v>
+      </c>
+      <c r="E18" s="7">
+        <v>350</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="7">
         <v>1000</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="1">
-        <v>350</v>
-      </c>
-      <c r="F19" s="1">
-        <v>2</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+        <v>21</v>
+      </c>
+      <c r="E19" s="7">
+        <v>350</v>
+      </c>
+      <c r="F19" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="7">
         <v>300</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="1">
-        <v>350</v>
-      </c>
-      <c r="F20" s="1">
-        <v>2</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+        <v>21</v>
+      </c>
+      <c r="E20" s="7">
+        <v>350</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="7">
         <v>1000</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="1">
-        <v>350</v>
-      </c>
-      <c r="F21" s="1">
-        <v>2</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+      <c r="E21" s="7">
+        <v>350</v>
+      </c>
+      <c r="F21" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="7">
         <v>300</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="1">
-        <v>350</v>
-      </c>
-      <c r="F22" s="1">
-        <v>2</v>
-      </c>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+      <c r="E22" s="7">
+        <v>350</v>
+      </c>
+      <c r="F22" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="7">
         <v>1000</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="1">
-        <v>350</v>
-      </c>
-      <c r="F23" s="1">
-        <v>2</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+      <c r="E23" s="7">
+        <v>350</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="7">
         <v>300</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="1">
-        <v>350</v>
-      </c>
-      <c r="F24" s="1">
-        <v>2</v>
-      </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+        <v>21</v>
+      </c>
+      <c r="E24" s="7">
+        <v>350</v>
+      </c>
+      <c r="F24" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="7">
         <v>800</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="1">
+        <v>21</v>
+      </c>
+      <c r="E25" s="7">
         <v>500</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="7">
         <v>11</v>
       </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    </row>
+    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="7">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="1">
+        <v>21</v>
+      </c>
+      <c r="E26" s="7">
         <v>800</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="7">
         <v>11</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
these changes get torque stand to stop after loop count complete
</commit_message>
<xml_diff>
--- a/upload_files/RTM_config.xlsx
+++ b/upload_files/RTM_config.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen.Garden\RTM\upload_files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E944F32-5CDD-4072-A72D-3BBA51D6B6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Config" sheetId="1" r:id="rId1"/>
-    <sheet name="Steps" sheetId="2" r:id="rId2"/>
+    <sheet r:id="rId1" sheetId="1" name="Config"/>
+    <sheet r:id="rId2" sheetId="2" name="Steps"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
   <si>
     <t>Step</t>
   </si>
@@ -65,6 +59,24 @@
     <t>CW</t>
   </si>
   <si>
+    <t>CCW</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>isHighSpeedGearBox</t>
+  </si>
+  <si>
+    <t>SPR</t>
+  </si>
+  <si>
+    <t>SPR_3</t>
+  </si>
+  <si>
     <t>Note:</t>
   </si>
   <si>
@@ -84,34 +96,14 @@
   </si>
   <si>
     <t>power.</t>
-  </si>
-  <si>
-    <t>CCW</t>
-  </si>
-  <si>
-    <t>Setting</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>isHighSpeedGearBox</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>SPR</t>
-  </si>
-  <si>
-    <t>SPR_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +121,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -160,40 +158,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="11">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -204,10 +209,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -245,71 +250,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -337,7 +342,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -360,11 +365,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -373,13 +378,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -389,7 +394,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -398,7 +403,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -407,7 +412,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -415,10 +420,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -483,103 +488,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="5" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>800</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="B9" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="B10" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="B11" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="B12" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="B13" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="2"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B15" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="7"/>
+      <c r="B16" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="2"/>
+      <c r="B18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -587,543 +610,541 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="7">
-        <v>1000</v>
+      <c r="C3" s="3">
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="3">
         <v>500</v>
       </c>
-      <c r="F3" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="7">
-        <v>300</v>
+      <c r="C4" s="3">
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="7">
-        <v>350</v>
-      </c>
-      <c r="F4" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="3">
+        <v>350</v>
+      </c>
+      <c r="F4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7">
-        <v>1000</v>
+      <c r="C5" s="3">
+        <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="7">
-        <v>350</v>
-      </c>
-      <c r="F5" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="3">
+        <v>350</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="7">
-        <v>300</v>
+      <c r="C6" s="3">
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="7">
-        <v>350</v>
-      </c>
-      <c r="F6" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="3">
+        <v>350</v>
+      </c>
+      <c r="F6" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="7">
-        <v>1000</v>
+      <c r="C7" s="3">
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="7">
-        <v>350</v>
-      </c>
-      <c r="F7" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="3">
+        <v>350</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7">
-        <v>300</v>
+      <c r="C8" s="3">
+        <v>60</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7">
-        <v>350</v>
-      </c>
-      <c r="F8" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="3">
+        <v>350</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7">
-        <v>1000</v>
+      <c r="C9" s="3">
+        <v>20</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="7">
-        <v>350</v>
-      </c>
-      <c r="F9" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="3">
+        <v>350</v>
+      </c>
+      <c r="F9" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7">
-        <v>300</v>
+      <c r="C10" s="3">
+        <v>40</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="7">
-        <v>350</v>
-      </c>
-      <c r="F10" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="3">
+        <v>350</v>
+      </c>
+      <c r="F10" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="7">
-        <v>1000</v>
+      <c r="C11" s="3">
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="7">
-        <v>350</v>
-      </c>
-      <c r="F11" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="3">
+        <v>350</v>
+      </c>
+      <c r="F11" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="3">
         <v>300</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="7">
-        <v>350</v>
-      </c>
-      <c r="F12" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="3">
+        <v>350</v>
+      </c>
+      <c r="F12" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="3">
         <v>800</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="3">
         <v>500</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="3">
         <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="3">
         <v>800</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="3">
         <v>1000</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="7">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3">
         <v>500</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="3">
         <v>300</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="7">
-        <v>350</v>
-      </c>
-      <c r="F16" s="7">
+        <v>14</v>
+      </c>
+      <c r="E16" s="3">
+        <v>350</v>
+      </c>
+      <c r="F16" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="3">
         <v>1000</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="7">
-        <v>350</v>
-      </c>
-      <c r="F17" s="7">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3">
+        <v>350</v>
+      </c>
+      <c r="F17" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="3">
         <v>300</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="7">
-        <v>350</v>
-      </c>
-      <c r="F18" s="7">
+        <v>14</v>
+      </c>
+      <c r="E18" s="3">
+        <v>350</v>
+      </c>
+      <c r="F18" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="3">
         <v>1000</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="7">
-        <v>350</v>
-      </c>
-      <c r="F19" s="7">
+        <v>14</v>
+      </c>
+      <c r="E19" s="3">
+        <v>350</v>
+      </c>
+      <c r="F19" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="3">
         <v>300</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="7">
-        <v>350</v>
-      </c>
-      <c r="F20" s="7">
+        <v>14</v>
+      </c>
+      <c r="E20" s="3">
+        <v>350</v>
+      </c>
+      <c r="F20" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="3">
         <v>1000</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="7">
-        <v>350</v>
-      </c>
-      <c r="F21" s="7">
+        <v>14</v>
+      </c>
+      <c r="E21" s="3">
+        <v>350</v>
+      </c>
+      <c r="F21" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="3">
         <v>300</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" s="7">
-        <v>350</v>
-      </c>
-      <c r="F22" s="7">
+        <v>14</v>
+      </c>
+      <c r="E22" s="3">
+        <v>350</v>
+      </c>
+      <c r="F22" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="3">
         <v>1000</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="7">
-        <v>350</v>
-      </c>
-      <c r="F23" s="7">
+        <v>14</v>
+      </c>
+      <c r="E23" s="3">
+        <v>350</v>
+      </c>
+      <c r="F23" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="3">
         <v>300</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7">
-        <v>350</v>
-      </c>
-      <c r="F24" s="7">
+        <v>14</v>
+      </c>
+      <c r="E24" s="3">
+        <v>350</v>
+      </c>
+      <c r="F24" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="3">
         <v>800</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="7">
+        <v>14</v>
+      </c>
+      <c r="E25" s="3">
         <v>500</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="3">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1">
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="3">
         <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="7">
+        <v>14</v>
+      </c>
+      <c r="E26" s="3">
         <v>800</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="3">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update profile and change to abs pos
</commit_message>
<xml_diff>
--- a/upload_files/RTM_config.xlsx
+++ b/upload_files/RTM_config.xlsx
@@ -1,40 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://trelleborg-my.sharepoint.com/personal/stephen_garden_trelleborg_com/Documents/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="11_694819EBBCC7D56918958E055A200F48E03D2733" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F34ECD7A-8AFD-4C37-BE72-4A228E58CF1B}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Config" sheetId="1" r:id="rId1"/>
-    <sheet name="Steps" sheetId="2" r:id="rId2"/>
+    <sheet r:id="rId1" sheetId="1" name="Config"/>
+    <sheet r:id="rId2" sheetId="2" name="Steps"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Step</t>
   </si>
@@ -42,6 +23,12 @@
     <t>Heat On/Off</t>
   </si>
   <si>
+    <t>Hold Step</t>
+  </si>
+  <si>
+    <t>Hold Duration</t>
+  </si>
+  <si>
     <t>Target Position</t>
   </si>
   <si>
@@ -57,6 +44,9 @@
     <t>True / False</t>
   </si>
   <si>
+    <t>secs</t>
+  </si>
+  <si>
     <t>deg</t>
   </si>
   <si>
@@ -66,6 +56,12 @@
     <t>rpm / s</t>
   </si>
   <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Setting</t>
   </si>
   <si>
@@ -102,9 +98,6 @@
     <t>power.</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Test:</t>
   </si>
   <si>
@@ -112,22 +105,14 @@
   </si>
   <si>
     <t>70°C</t>
-  </si>
-  <si>
-    <t>Hold Step</t>
-  </si>
-  <si>
-    <t>Hold Duration</t>
-  </si>
-  <si>
-    <t>secs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +123,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -176,48 +167,62 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -225,10 +230,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -266,71 +271,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -358,7 +363,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -381,11 +386,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -394,13 +399,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -410,7 +415,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -419,7 +424,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -428,7 +433,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -436,10 +441,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -504,127 +509,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B2" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1">
         <v>600</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="7">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6">
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="2"/>
-      <c r="B5" s="7"/>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="7"/>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="B7" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="B8" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="B10" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="7"/>
-    </row>
-    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="B12" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="2"/>
+      <c r="B13" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="2"/>
+      <c r="B14" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="7"/>
-    </row>
-    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="B16" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1"/>
     </row>
@@ -634,302 +633,341 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="12.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="b">
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
+      <c r="E3" s="4">
         <v>62.37</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="7">
         <v>94.5</v>
       </c>
       <c r="G3" s="1">
         <v>945</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="7">
         <v>0.1</v>
       </c>
-      <c r="E4" s="9">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
+      <c r="E4" s="4">
+        <v>62.37</v>
+      </c>
+      <c r="F4" s="6">
         <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="b">
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6">
         <v>0</v>
       </c>
-      <c r="C5" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9">
+      <c r="E5" s="4">
         <v>-62.37</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="7">
         <v>94.5</v>
       </c>
       <c r="G5" s="1">
         <v>945</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7">
         <v>0.1</v>
       </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
+      <c r="E6" s="4">
+        <v>-62.37</v>
+      </c>
+      <c r="F6" s="6">
         <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="5"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="5"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
       <c r="G26" s="1"/>
     </row>
   </sheetData>

</xml_diff>